<commit_message>
Se agregaron los datos de pruebas
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdina\Documents\GitHub\ProyectoDominoBacktracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilberth\Documents\Github\ProyectoDominoBacktracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1164252-DD1A-46C3-841A-2A85CE81A997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E73254C-1D50-4902-8A70-0025F77B370C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{46AFC8A5-E767-48AF-8E32-FC201D985F49}"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="9915" windowHeight="8325" activeTab="1" xr2:uid="{46AFC8A5-E767-48AF-8E32-FC201D985F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de actividades faltantes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Actividad</t>
   </si>
@@ -86,6 +86,27 @@
   </si>
   <si>
     <t>15/9/2021 - 20/9/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>5.46580211E10</t>
+  </si>
+  <si>
+    <t>1.214639335E11</t>
+  </si>
+  <si>
+    <t>5.40886859E10</t>
+  </si>
+  <si>
+    <t>1.06704465E10</t>
+  </si>
+  <si>
+    <t>1.643519309E11</t>
+  </si>
+  <si>
+    <t>2.5464494523E12</t>
   </si>
 </sst>
 </file>
@@ -203,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,6 +251,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -374,25 +396,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>180860</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>408700</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>623080</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1663840</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>32847940</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1965873360</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>267916068820</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -883,25 +905,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>52300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>351460</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>542100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1395600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>19725340</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>180961180</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2997673540</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2433,15 +2455,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>552450</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2500,13 +2522,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2567,15 +2589,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>552450</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2634,13 +2656,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2701,13 +2723,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2768,13 +2790,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2835,13 +2857,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2902,13 +2924,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>8</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2969,13 +2991,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3036,15 +3058,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>350520</xdr:colOff>
+          <xdr:colOff>352425</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>0</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>552450</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>200025</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3480,18 +3502,18 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="39.88671875" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -3502,7 +3524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -3511,7 +3533,7 @@
         <v>44436</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -3520,7 +3542,7 @@
         <v>44437</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -3529,7 +3551,7 @@
         <v>44437</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -3538,7 +3560,7 @@
         <v>44439</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -3547,7 +3569,7 @@
         <v>44439</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -3556,7 +3578,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -3565,7 +3587,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="2" t="s">
         <v>5</v>
@@ -3574,7 +3596,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="2" t="s">
         <v>6</v>
@@ -3583,7 +3605,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="2" t="s">
         <v>7</v>
@@ -3606,15 +3628,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>198120</xdr:rowOff>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3628,13 +3650,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -3650,15 +3672,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>198120</xdr:rowOff>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3672,13 +3694,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -3694,13 +3716,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -3716,13 +3738,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -3738,13 +3760,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -3760,13 +3782,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>8</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -3782,13 +3804,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>9</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -3804,15 +3826,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>350520</xdr:colOff>
+                    <xdr:colOff>352425</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>7620</xdr:rowOff>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>0</xdr:col>
-                    <xdr:colOff>556260</xdr:colOff>
+                    <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>198120</xdr:rowOff>
+                    <xdr:rowOff>200025</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3829,35 +3851,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9C10FC-6A69-47AC-A1E1-32326C60F61E}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.109375" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="18.88671875" customWidth="1"/>
+    <col min="2" max="3" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
       <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
@@ -3865,101 +3887,326 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="L2" t="e">
+      <c r="B2">
+        <v>216000</v>
+      </c>
+      <c r="C2">
+        <v>146200</v>
+      </c>
+      <c r="D2">
+        <v>168400</v>
+      </c>
+      <c r="E2">
+        <v>171900</v>
+      </c>
+      <c r="F2">
+        <v>201800</v>
+      </c>
+      <c r="G2">
+        <v>225800</v>
+      </c>
+      <c r="H2">
+        <v>11500</v>
+      </c>
+      <c r="I2">
+        <v>10000</v>
+      </c>
+      <c r="J2">
+        <v>8100</v>
+      </c>
+      <c r="K2">
+        <v>6100</v>
+      </c>
+      <c r="L2">
         <f>AVERAGE(B2:F2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M2" t="e">
+        <v>180860</v>
+      </c>
+      <c r="M2">
         <f>AVERAGE(G2:K2)</f>
-        <v>#DIV/0!</v>
+        <v>52300</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="L3" t="e">
+      <c r="B3">
+        <v>373100</v>
+      </c>
+      <c r="C3">
+        <v>461300</v>
+      </c>
+      <c r="D3">
+        <v>426100</v>
+      </c>
+      <c r="E3">
+        <v>180400</v>
+      </c>
+      <c r="F3">
+        <v>602600</v>
+      </c>
+      <c r="G3">
+        <v>156300</v>
+      </c>
+      <c r="H3">
+        <v>469100</v>
+      </c>
+      <c r="I3">
+        <v>401300</v>
+      </c>
+      <c r="J3">
+        <v>349100</v>
+      </c>
+      <c r="K3">
+        <v>381500</v>
+      </c>
+      <c r="L3">
         <f>AVERAGE(B3:F3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M3" t="e">
+        <v>408700</v>
+      </c>
+      <c r="M3">
         <f>AVERAGE(G3:K3)</f>
-        <v>#DIV/0!</v>
+        <v>351460</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="L4" t="e">
+      <c r="B4">
+        <v>549300</v>
+      </c>
+      <c r="C4">
+        <v>754100</v>
+      </c>
+      <c r="D4">
+        <v>753800</v>
+      </c>
+      <c r="E4">
+        <v>736100</v>
+      </c>
+      <c r="F4">
+        <v>322100</v>
+      </c>
+      <c r="G4">
+        <v>542400</v>
+      </c>
+      <c r="H4" s="10">
+        <v>493900</v>
+      </c>
+      <c r="I4">
+        <v>467400</v>
+      </c>
+      <c r="J4" s="10">
+        <v>437500</v>
+      </c>
+      <c r="K4">
+        <v>769300</v>
+      </c>
+      <c r="L4">
         <f>AVERAGE(B4:F4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M4" t="e">
+        <v>623080</v>
+      </c>
+      <c r="M4">
         <f t="shared" ref="M4:M32" si="0">AVERAGE(G4:K4)</f>
-        <v>#DIV/0!</v>
+        <v>542100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="L5" t="e">
+      <c r="B5" s="10">
+        <v>2269600</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1271100</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1905600</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1681600</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1191300</v>
+      </c>
+      <c r="G5" s="10">
+        <v>419400</v>
+      </c>
+      <c r="H5" s="10">
+        <v>2441700</v>
+      </c>
+      <c r="I5" s="10">
+        <v>907700</v>
+      </c>
+      <c r="J5" s="10">
+        <v>963300</v>
+      </c>
+      <c r="K5" s="10">
+        <v>2245900</v>
+      </c>
+      <c r="L5">
         <f t="shared" ref="L5:L32" si="1">AVERAGE(B5:F5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" t="e">
+        <v>1663840</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>1395600</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="L6" t="e">
+      <c r="B6" s="10">
+        <v>32617900</v>
+      </c>
+      <c r="C6" s="10">
+        <v>32385800</v>
+      </c>
+      <c r="D6" s="10">
+        <v>27827400</v>
+      </c>
+      <c r="E6" s="10">
+        <v>29895500</v>
+      </c>
+      <c r="F6" s="10">
+        <v>41513100</v>
+      </c>
+      <c r="G6" s="10">
+        <v>4427500</v>
+      </c>
+      <c r="H6" s="10">
+        <v>56222500</v>
+      </c>
+      <c r="I6" s="10">
+        <v>14717400</v>
+      </c>
+      <c r="J6" s="10">
+        <v>2224400</v>
+      </c>
+      <c r="K6" s="10">
+        <v>21034900</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M6" t="e">
+        <v>32847940</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>19725340</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="L7" t="e">
+      <c r="B7" s="10">
+        <v>1933673800</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2071326500</v>
+      </c>
+      <c r="D7" s="10">
+        <v>1952791200</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1938544900</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1933030400</v>
+      </c>
+      <c r="G7" s="10">
+        <v>260353000</v>
+      </c>
+      <c r="H7" s="10">
+        <v>16206000</v>
+      </c>
+      <c r="I7" s="10">
+        <v>195705600</v>
+      </c>
+      <c r="J7" s="10">
+        <v>255979300</v>
+      </c>
+      <c r="K7" s="10">
+        <v>176562000</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" t="e">
+        <v>1965873360</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>180961180</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="L8" t="e">
+      <c r="B8" s="10">
+        <v>272288491900</v>
+      </c>
+      <c r="C8" s="10">
+        <v>268872935400</v>
+      </c>
+      <c r="D8" s="10">
+        <v>264121187400</v>
+      </c>
+      <c r="E8" s="10">
+        <v>266763112200</v>
+      </c>
+      <c r="F8" s="10">
+        <v>267534617200</v>
+      </c>
+      <c r="G8" s="10">
+        <v>1909830000</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1450962800</v>
+      </c>
+      <c r="I8" s="10">
+        <v>8753417600</v>
+      </c>
+      <c r="J8" s="10">
+        <v>2021460300</v>
+      </c>
+      <c r="K8" s="10">
+        <v>852697000</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" t="e">
+        <v>267916068820</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>2997673540</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
       <c r="L9" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -3969,10 +4216,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
       <c r="L10" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -3982,7 +4235,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3995,7 +4248,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4008,7 +4261,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4021,7 +4274,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4034,7 +4287,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4047,7 +4300,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4060,7 +4313,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -4073,7 +4326,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4086,7 +4339,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -4099,7 +4352,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -4112,7 +4365,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -4125,7 +4378,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -4138,7 +4391,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -4151,7 +4404,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -4164,7 +4417,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -4177,7 +4430,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -4190,7 +4443,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -4203,7 +4456,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -4216,7 +4469,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -4229,7 +4482,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -4242,7 +4495,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4255,7 +4508,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Agregado la grafica de medicion analitica de BT
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gilberth\Documents\Github\ProyectoDominoBacktracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E73254C-1D50-4902-8A70-0025F77B370C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10DA04F-5FF3-4F76-A319-68FA9F9C4739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="855" windowWidth="9915" windowHeight="8325" activeTab="1" xr2:uid="{46AFC8A5-E767-48AF-8E32-FC201D985F49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{46AFC8A5-E767-48AF-8E32-FC201D985F49}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de actividades faltantes" sheetId="1" r:id="rId1"/>
     <sheet name="Plan de pruebas" sheetId="2" r:id="rId2"/>
+    <sheet name="Grafica BT Analtica" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Actividad</t>
   </si>
@@ -107,6 +108,9 @@
   </si>
   <si>
     <t>2.5464494523E12</t>
+  </si>
+  <si>
+    <t>Backtracking</t>
   </si>
 </sst>
 </file>
@@ -224,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,6 +256,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1296,6 +1303,567 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Backtracking Algorithm</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Grafica BT Analtica'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Grafica BT Analtica'!$A$2:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Grafica BT Analtica'!$B$2:$B$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>65536</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>131072</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>524288</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1048576</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4194304</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8388608</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33554432</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>67108864</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>134217728</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>268435456</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>536870912</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1073741824</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-A922-45E0-BE19-81256C192945}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="513617880"/>
+        <c:axId val="513618208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="513617880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513618208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="513618208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513617880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1376,6 +1944,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2404,6 +3012,508 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="248">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3163,16 +4273,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>735153</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>51922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>580537</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>51922</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3194,6 +4304,49 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9CBBEEF-A053-4302-AD7D-A3D4326E9B96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3851,8 +5004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9C10FC-6A69-47AC-A1E1-32326C60F61E}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="A9" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3866,20 +5019,20 @@
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
       <c r="L1" s="3" t="s">
         <v>16</v>
       </c>
@@ -4529,4 +5682,281 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC36ADD6-9E27-4943-87DC-E419107BCCD2}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>32768</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>131072</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>262144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>524288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>1048576</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>2097152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>4194304</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>8388608</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>33554432</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>67108864</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>134217728</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>268435456</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>536870912</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>1073741824</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>